<commit_message>
lab entry in new changes commit
</commit_message>
<xml_diff>
--- a/SunriseLabWeb/Content/images/LabEntry_Format.xlsx
+++ b/SunriseLabWeb/Content/images/LabEntry_Format.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hardik Projects\Sunrise_NewLab\SunriseLabWeb\Content\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344A29D6-FDE1-4982-809A-98A6F7538E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2F085C-1C1A-483D-A408-4BF36650725D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FA0BA61D-0729-4998-A5B2-02679023B6B9}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="StoneSelection" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">StoneSelection!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">StoneSelection!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,33 +28,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Status</t>
   </si>
   <si>
-    <t>Supplier Cost Disc(%)</t>
-  </si>
-  <si>
-    <t>Offer Disc(%)</t>
-  </si>
-  <si>
-    <t>HIYU00036035</t>
-  </si>
-  <si>
     <t>HIYU00040082</t>
   </si>
   <si>
     <t>Ref No</t>
   </si>
   <si>
-    <t>HIVU00040082</t>
-  </si>
-  <si>
-    <t>HIYU00039318</t>
-  </si>
-  <si>
     <t>Confirm</t>
+  </si>
+  <si>
+    <t>Supplier Cost Value($)</t>
+  </si>
+  <si>
+    <t>QC Require</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>QC Pending</t>
+  </si>
+  <si>
+    <t>QC Reject</t>
+  </si>
+  <si>
+    <t>Bidded</t>
+  </si>
+  <si>
+    <t>Hold</t>
+  </si>
+  <si>
+    <t>HIYU00040084</t>
+  </si>
+  <si>
+    <t>HIYU00040083</t>
+  </si>
+  <si>
+    <t>HIYU00040086</t>
+  </si>
+  <si>
+    <t>HIYU00040087</t>
+  </si>
+  <si>
+    <t>HIYU00040088</t>
+  </si>
+  <si>
+    <t>HIYO00040088</t>
+  </si>
+  <si>
+    <t>Sunrise Value($)</t>
   </si>
 </sst>
 </file>
@@ -412,134 +442,153 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{944EBE10-BD9C-446A-91D2-F3CB9AD105B1}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2">
+        <v>100</v>
+      </c>
+      <c r="E2" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D3" s="2">
+        <v>200</v>
+      </c>
+      <c r="E3" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>300</v>
+      </c>
+      <c r="E4" s="2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2">
-        <v>-41.08</v>
-      </c>
-      <c r="D2" s="2">
-        <v>-40.08</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2">
-        <v>-37.94</v>
-      </c>
-      <c r="D3" s="2">
-        <v>-36.94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="D5" s="2">
+        <v>400</v>
+      </c>
+      <c r="E5" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2">
+        <v>500</v>
+      </c>
+      <c r="E6" s="2">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="2">
+        <v>600</v>
+      </c>
+      <c r="E7" s="2">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2">
-        <v>-37.94</v>
-      </c>
-      <c r="D4" s="2">
-        <v>-36.94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2">
-        <v>-37.94</v>
-      </c>
-      <c r="D5" s="2">
-        <v>-36.94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="2">
-        <v>-37.94</v>
-      </c>
-      <c r="D6" s="2">
-        <v>-36.94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="2">
-        <v>-37.94</v>
-      </c>
-      <c r="D7" s="2">
-        <v>-36.94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="2">
-        <v>-37.94</v>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D8" s="2">
-        <v>-36.94</v>
+        <v>700</v>
+      </c>
+      <c r="E8" s="2">
+        <v>800</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1" xr:uid="{944EBE10-BD9C-446A-91D2-F3CB9AD105B1}"/>
+  <autoFilter ref="A1:E1" xr:uid="{944EBE10-BD9C-446A-91D2-F3CB9AD105B1}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>